<commit_message>
fixed cdc data graphs both columns now somewhat fixed county outputs only 1 pie chart
</commit_message>
<xml_diff>
--- a/Case Data Services/CountyDataByState.xlsx
+++ b/Case Data Services/CountyDataByState.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/TeamPi-P2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/TeamPi-P2/Case Data Services/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{04189930-62D4-4FA5-A872-75AB556CE125}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5D979183-C2D7-4209-B9F0-7D99EB2E7E0A}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{5736CDB6-B236-43D3-951C-4E9597EC4C72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{719BCE46-69F6-4DAD-880C-B8BB33103AAE}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="880" windowWidth="11780" windowHeight="9320" xr2:uid="{AB3FD4F4-44CB-4A46-8B44-90288A03EF19}"/>
+    <workbookView xWindow="7340" yWindow="880" windowWidth="11780" windowHeight="9320" xr2:uid="{43FC9ABF-BDC4-4FC1-8C95-F6C7E607D9B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Texas Yesterday" sheetId="2" r:id="rId1"/>
@@ -892,6 +892,1670 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Total Cases in Texas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Texas Yesterday'!$A$3:$A$256</c:f>
+              <c:strCache>
+                <c:ptCount val="254"/>
+                <c:pt idx="0">
+                  <c:v>Harris</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Dallas</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tarrant</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>El Paso</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Bexar</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Hidalgo</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Travis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Lubbock</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Cameron</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Collin</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Nueces</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Denton</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>Fort Bend</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>Webb</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>Montgomery</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>Galveston</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>Brazoria</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>McLennan</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>Williamson</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>Potter</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>Brazos</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>Randall</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>Jefferson</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>Midland</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>Smith</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>Tom Green</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>Ector</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>Bell</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>Hays</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>Taylor</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>Ellis</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>Wichita</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>Johnson</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>Victoria</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>Walker</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>Gregg</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>Kaufman</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>Guadalupe</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>Maverick</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>Comal</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>Starr</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>Grayson</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>Hale</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>Parker</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>Angelina</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>Val Verde</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>Anderson</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>Rockwall</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>Hunt</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>Lamar</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>Navarro</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>Coryell</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>Orange</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>Liberty</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>Bowie</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>Henderson</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>Bastrop</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>Bee</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>Jim Wells</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>Chambers</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>Nacogdoches</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>Medina</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>Howard</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>San Patricio</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>Caldwell</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>Atascosa</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>Titus</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>Cherokee</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>Deaf Smith</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>Wise</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>Van Zandt</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>Brown</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>Wharton</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>Moore</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>Hood</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>Jones</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>Hardin</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>Scurry</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>Polk</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>Lavaca</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>Wood</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>Young</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>Burnet</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>Grimes</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>Willacy</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>Erath</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>Hockley</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>Gray</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>Gonzales</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>Wilson</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>Matagorda</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>Harrison</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>Hill</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>Rusk</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>DeWitt</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>Kleberg</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>Dawson</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>Waller</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>Kerr</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>Uvalde</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>Frio</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>Palo Pinto</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>Calhoun</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>Andrews</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>Karnes</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>Fannin</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>Lamb</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>Washington</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>Gaines</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>Cooke</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>Terry</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>Fayette</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>Reeves</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>Madison</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>Kendall</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>Hopkins</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>Childress</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>Jackson</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>Falls</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>Pecos</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>Limestone</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>Cass</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>Dallam</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>Nolan</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>Gillespie</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>Parmer</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>Wilbarger</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>Comanche</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>Hutchinson</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>Burleson</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>Zavala</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>Milam</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>Brewster</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>Montague</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>Colorado</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>Upshur</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>Austin</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>Duval</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>Yoakum</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>Shelby</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>Houston</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>Ochiltree</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>Jasper</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>Panola</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>Bosque</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>Freestone</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>Robertson</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>Zapata</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>Hartley</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>Bailey</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>Castro</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>Lee</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>Presidio</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>Llano</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>Camp</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>Leon</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>Live Oak</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>Ward</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>Somervell</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>Aransas</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>Brooks</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>Lampasas</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>La Salle</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>Dimmit</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>Eastland</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>San Augustine</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>Runnels</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>Refugio</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>Lynn</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>Mitchell</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>Rains</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>Stephens</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>McCulloch</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>Tyler</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>Clay</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>San Saba</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>Bandera</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>Crockett</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>Hamilton</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>Winkler</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>Swisher</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>Morris</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>San Jacinto</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>Crane</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>Archer</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>Franklin</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>Hemphill</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>Jack</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>Martin</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>Hansford</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>Wheeler</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>Goliad</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>Trinity</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>Reagan</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>Hudspeth</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>Red River</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>Sutton</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>Callahan</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>Culberson</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>Jim Hogg</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>Coke</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>Newton</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>Floyd</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>Marion</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>Blanco</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>Coleman</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>Crosby</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>Garza</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>Fisher</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>Cochran</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>Mills</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>Baylor</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>Real</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>Lipscomb</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>Schleicher</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>Mason</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>Kimble</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>Concho</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>Sabine</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>Knox</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>Menard</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>Donley</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>Edwards</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>Carson</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>Haskell</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>Sherman</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>Hardeman</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>Kinney</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>Upton</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>Hall</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>Jeff Davis</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>Dickens</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>Cottle</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>Shackelford</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>Delta</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>Armstrong</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>Oldham</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>Glasscock</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>Briscoe</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>Collingsworth</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>Sterling</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>Foard</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>Irion</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>McMullen</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>Roberts</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>Stonewall</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>Kent</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>Terrell</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>Throckmorton</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>Motley</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>Kenedy</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>Borden</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>King</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>Loving</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Texas Yesterday'!$B$3:$B$256</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="254"/>
+                <c:pt idx="0">
+                  <c:v>187932</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>134793</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>95989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>85318</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>78411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>42844</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>37898</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31858</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>25855</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25566</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23276</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20440</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19703</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16982</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14691</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>14154</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>14029</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13574</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12360</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10858</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10443</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10187</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9935</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9393</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9013</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8873</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8443</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7963</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7860</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>6828</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6818</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5327</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5007</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4991</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4930</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4870</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4869</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4823</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4508</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4352</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4290</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4052</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3868</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3571</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3220</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3167</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2948</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2740</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2675</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2626</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2551</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2530</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2520</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2497</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2451</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2274</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2020</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1965</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1964</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1957</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1928</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1883</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1873</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1862</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1831</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1752</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1748</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1738</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1673</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1667</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1650</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1631</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1611</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1604</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1594</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1570</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1539</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1473</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1441</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1426</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1401</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1378</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1353</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1338</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1319</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1292</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1289</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>1286</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1269</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1234</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1230</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>1211</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1205</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>1183</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1178</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1171</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>1165</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>1161</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1122</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>1090</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1019</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>1018</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1003</c:v>
+                </c:pt>
+                <c:pt idx="105" formatCode="General">
+                  <c:v>994</c:v>
+                </c:pt>
+                <c:pt idx="106" formatCode="General">
+                  <c:v>986</c:v>
+                </c:pt>
+                <c:pt idx="107" formatCode="General">
+                  <c:v>958</c:v>
+                </c:pt>
+                <c:pt idx="108" formatCode="General">
+                  <c:v>936</c:v>
+                </c:pt>
+                <c:pt idx="109" formatCode="General">
+                  <c:v>934</c:v>
+                </c:pt>
+                <c:pt idx="110" formatCode="General">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="111" formatCode="General">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="112" formatCode="General">
+                  <c:v>868</c:v>
+                </c:pt>
+                <c:pt idx="113" formatCode="General">
+                  <c:v>867</c:v>
+                </c:pt>
+                <c:pt idx="114" formatCode="General">
+                  <c:v>866</c:v>
+                </c:pt>
+                <c:pt idx="115" formatCode="General">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="116" formatCode="General">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="117" formatCode="General">
+                  <c:v>825</c:v>
+                </c:pt>
+                <c:pt idx="118" formatCode="General">
+                  <c:v>803</c:v>
+                </c:pt>
+                <c:pt idx="119" formatCode="General">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="120" formatCode="General">
+                  <c:v>786</c:v>
+                </c:pt>
+                <c:pt idx="121" formatCode="General">
+                  <c:v>747</c:v>
+                </c:pt>
+                <c:pt idx="122" formatCode="General">
+                  <c:v>742</c:v>
+                </c:pt>
+                <c:pt idx="123" formatCode="General">
+                  <c:v>722</c:v>
+                </c:pt>
+                <c:pt idx="124" formatCode="General">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="125" formatCode="General">
+                  <c:v>704</c:v>
+                </c:pt>
+                <c:pt idx="126" formatCode="General">
+                  <c:v>689</c:v>
+                </c:pt>
+                <c:pt idx="127" formatCode="General">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="128" formatCode="General">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="129" formatCode="General">
+                  <c:v>657</c:v>
+                </c:pt>
+                <c:pt idx="130" formatCode="General">
+                  <c:v>651</c:v>
+                </c:pt>
+                <c:pt idx="131" formatCode="General">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="132" formatCode="General">
+                  <c:v>637</c:v>
+                </c:pt>
+                <c:pt idx="133" formatCode="General">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="134" formatCode="General">
+                  <c:v>623</c:v>
+                </c:pt>
+                <c:pt idx="135" formatCode="General">
+                  <c:v>606</c:v>
+                </c:pt>
+                <c:pt idx="136" formatCode="General">
+                  <c:v>604</c:v>
+                </c:pt>
+                <c:pt idx="137" formatCode="General">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="138" formatCode="General">
+                  <c:v>601</c:v>
+                </c:pt>
+                <c:pt idx="139" formatCode="General">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="140" formatCode="General">
+                  <c:v>574</c:v>
+                </c:pt>
+                <c:pt idx="141" formatCode="General">
+                  <c:v>554</c:v>
+                </c:pt>
+                <c:pt idx="142" formatCode="General">
+                  <c:v>547</c:v>
+                </c:pt>
+                <c:pt idx="143" formatCode="General">
+                  <c:v>539</c:v>
+                </c:pt>
+                <c:pt idx="144" formatCode="General">
+                  <c:v>531</c:v>
+                </c:pt>
+                <c:pt idx="145" formatCode="General">
+                  <c:v>513</c:v>
+                </c:pt>
+                <c:pt idx="146" formatCode="General">
+                  <c:v>508</c:v>
+                </c:pt>
+                <c:pt idx="147" formatCode="General">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="148" formatCode="General">
+                  <c:v>476</c:v>
+                </c:pt>
+                <c:pt idx="149" formatCode="General">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="150" formatCode="General">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="151" formatCode="General">
+                  <c:v>459</c:v>
+                </c:pt>
+                <c:pt idx="152" formatCode="General">
+                  <c:v>458</c:v>
+                </c:pt>
+                <c:pt idx="153" formatCode="General">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="154" formatCode="General">
+                  <c:v>449</c:v>
+                </c:pt>
+                <c:pt idx="155" formatCode="General">
+                  <c:v>446</c:v>
+                </c:pt>
+                <c:pt idx="156" formatCode="General">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="157" formatCode="General">
+                  <c:v>421</c:v>
+                </c:pt>
+                <c:pt idx="158" formatCode="General">
+                  <c:v>415</c:v>
+                </c:pt>
+                <c:pt idx="159" formatCode="General">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="160" formatCode="General">
+                  <c:v>399</c:v>
+                </c:pt>
+                <c:pt idx="161" formatCode="General">
+                  <c:v>394</c:v>
+                </c:pt>
+                <c:pt idx="162" formatCode="General">
+                  <c:v>392</c:v>
+                </c:pt>
+                <c:pt idx="163" formatCode="General">
+                  <c:v>372</c:v>
+                </c:pt>
+                <c:pt idx="164" formatCode="General">
+                  <c:v>368</c:v>
+                </c:pt>
+                <c:pt idx="165" formatCode="General">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="166" formatCode="General">
+                  <c:v>358</c:v>
+                </c:pt>
+                <c:pt idx="167" formatCode="General">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="168" formatCode="General">
+                  <c:v>345</c:v>
+                </c:pt>
+                <c:pt idx="169" formatCode="General">
+                  <c:v>338</c:v>
+                </c:pt>
+                <c:pt idx="170" formatCode="General">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="171" formatCode="General">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="172" formatCode="General">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="173" formatCode="General">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="174" formatCode="General">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="175" formatCode="General">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="176" formatCode="General">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="177" formatCode="General">
+                  <c:v>297</c:v>
+                </c:pt>
+                <c:pt idx="178" formatCode="General">
+                  <c:v>294</c:v>
+                </c:pt>
+                <c:pt idx="179" formatCode="General">
+                  <c:v>283</c:v>
+                </c:pt>
+                <c:pt idx="180" formatCode="General">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="181" formatCode="General">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="182" formatCode="General">
+                  <c:v>257</c:v>
+                </c:pt>
+                <c:pt idx="183" formatCode="General">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="184" formatCode="General">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="185" formatCode="General">
+                  <c:v>249</c:v>
+                </c:pt>
+                <c:pt idx="186" formatCode="General">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="187" formatCode="General">
+                  <c:v>247</c:v>
+                </c:pt>
+                <c:pt idx="188" formatCode="General">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="189" formatCode="General">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="190" formatCode="General">
+                  <c:v>236</c:v>
+                </c:pt>
+                <c:pt idx="191" formatCode="General">
+                  <c:v>235</c:v>
+                </c:pt>
+                <c:pt idx="192" formatCode="General">
+                  <c:v>228</c:v>
+                </c:pt>
+                <c:pt idx="193" formatCode="General">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="194" formatCode="General">
+                  <c:v>226</c:v>
+                </c:pt>
+                <c:pt idx="195" formatCode="General">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="196" formatCode="General">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="197" formatCode="General">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="198" formatCode="General">
+                  <c:v>216</c:v>
+                </c:pt>
+                <c:pt idx="199" formatCode="General">
+                  <c:v>213</c:v>
+                </c:pt>
+                <c:pt idx="200" formatCode="General">
+                  <c:v>201</c:v>
+                </c:pt>
+                <c:pt idx="201" formatCode="General">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="202" formatCode="General">
+                  <c:v>186</c:v>
+                </c:pt>
+                <c:pt idx="203" formatCode="General">
+                  <c:v>184</c:v>
+                </c:pt>
+                <c:pt idx="204" formatCode="General">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="205" formatCode="General">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="206" formatCode="General">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="207" formatCode="General">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="208" formatCode="General">
+                  <c:v>159</c:v>
+                </c:pt>
+                <c:pt idx="209" formatCode="General">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="210" formatCode="General">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="211" formatCode="General">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="212" formatCode="General">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="213" formatCode="General">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="214" formatCode="General">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="215" formatCode="General">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="216" formatCode="General">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="217" formatCode="General">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="218" formatCode="General">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="219" formatCode="General">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="220" formatCode="General">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="221" formatCode="General">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="222" formatCode="General">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="223" formatCode="General">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="224" formatCode="General">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="225" formatCode="General">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="226" formatCode="General">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="227" formatCode="General">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="228" formatCode="General">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="229" formatCode="General">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="230" formatCode="General">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="231" formatCode="General">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="232" formatCode="General">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="233" formatCode="General">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="234" formatCode="General">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="235" formatCode="General">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="236" formatCode="General">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="237" formatCode="General">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="238" formatCode="General">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="239" formatCode="General">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="240" formatCode="General">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="241" formatCode="General">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="242" formatCode="General">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="243" formatCode="General">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="244" formatCode="General">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="245" formatCode="General">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="246" formatCode="General">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="247" formatCode="General">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="248" formatCode="General">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="249" formatCode="General">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="250" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="251" formatCode="General">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="252" formatCode="General">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="253" formatCode="General">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-250F-457B-AEA6-049785F2D575}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3ADB6A3B-6CDD-4F5A-AA1B-5DCAFA235069}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1190,10 +2854,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4266B5B6-1593-4EAB-85B0-732340B5D616}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22BF841D-0586-411B-9714-5C235019C489}">
   <dimension ref="A1:G258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -5354,11 +7020,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A412340E-6CF6-43B8-8274-A6998894B232}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{449A6EAC-8084-4BF9-828F-B03966CE00CF}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>